<commit_message>
added more object attributes to pawtucket details page template
</commit_message>
<xml_diff>
--- a/support/dennis_export/mappings/dennis_spreadsheet_mapping.xlsx
+++ b/support/dennis_export/mappings/dennis_spreadsheet_mapping.xlsx
@@ -423,15 +423,15 @@
     <t>Object name</t>
   </si>
   <si>
-    <t>{
-    "context" : "ca_entities",
-    "restrictToRelationshipTypes" : ["donor", "lender", "vendor", "trader", "transfer_party"],
-    "delimiter" : "; "
-}</t>
-  </si>
-  <si>
     <t>Related entities (Donor/Lender/Vendor/Transfer party)
 known bug: even if there are multiple entities, only returns last one</t>
+  </si>
+  <si>
+    <t>{
+    "context": "ca_entities",
+    "restrictToRelationshipTypes": ["donor", "lender", "vendor", "trader", "transfer_party"],
+    "delimiter": "; "
+}</t>
   </si>
 </sst>
 </file>
@@ -783,8 +783,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -957,10 +957,10 @@
         <v>78</v>
       </c>
       <c r="F9" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="G9" s="8" t="s">
         <v>132</v>
-      </c>
-      <c r="G9" s="8" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>